<commit_message>
SUMIF now copes with criteria ranges that are different in size from sum ranges
</commit_message>
<xml_diff>
--- a/examples/rangesinsteadofcells.xlsx
+++ b/examples/rangesinsteadofcells.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="6">
   <si>
     <t>F</t>
   </si>
@@ -29,6 +29,15 @@
   </si>
   <si>
     <t>D</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -83,8 +92,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="27">
+  <cellStyleXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -119,7 +130,7 @@
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
-  <cellStyles count="27">
+  <cellStyles count="29">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -133,6 +144,7 @@
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -146,6 +158,7 @@
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -475,10 +488,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B6:N22"/>
+  <dimension ref="B6:N34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -763,7 +776,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="3:8">
+    <row r="18" spans="3:10">
       <c r="C18">
         <f t="shared" ref="C18:G18" si="5">10/$C$6:$H$6</f>
         <v>10</v>
@@ -789,33 +802,33 @@
         <v>1.6666666666666667</v>
       </c>
     </row>
-    <row r="19" spans="3:8">
+    <row r="19" spans="3:10">
       <c r="C19">
-        <f>$C$6:$H$6</f>
+        <f t="shared" ref="C19:H19" si="6">$C$6:$H$6</f>
         <v>1</v>
       </c>
       <c r="D19">
-        <f>$C$6:$H$6</f>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="E19">
-        <f>$C$6:$H$6</f>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="F19">
-        <f>$C$6:$H$6</f>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="G19">
-        <f>$C$6:$H$6</f>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="H19">
-        <f>$C$6:$H$6</f>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="3:8">
+    <row r="22" spans="3:10">
       <c r="C22" t="e">
         <f>$C$7:$H$8</f>
         <v>#VALUE!</v>
@@ -830,6 +843,98 @@
       </c>
       <c r="F22" t="e">
         <f>$C$6:$E$6+$E$7:$H$7</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="28" spans="3:10">
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="F28" t="s">
+        <v>3</v>
+      </c>
+      <c r="H28">
+        <v>1</v>
+      </c>
+      <c r="I28" t="s">
+        <v>3</v>
+      </c>
+      <c r="J28" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="3:10">
+      <c r="E29">
+        <v>2</v>
+      </c>
+      <c r="F29" t="s">
+        <v>4</v>
+      </c>
+      <c r="H29">
+        <v>2</v>
+      </c>
+      <c r="I29" t="s">
+        <v>4</v>
+      </c>
+      <c r="J29" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="3:10">
+      <c r="E30">
+        <v>3</v>
+      </c>
+      <c r="F30" t="s">
+        <v>3</v>
+      </c>
+      <c r="H30">
+        <v>3000</v>
+      </c>
+      <c r="I30" t="s">
+        <v>3</v>
+      </c>
+      <c r="J30" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="3:10">
+      <c r="E31">
+        <v>4</v>
+      </c>
+      <c r="F31" t="s">
+        <v>4</v>
+      </c>
+      <c r="H31">
+        <v>4</v>
+      </c>
+      <c r="I31" t="s">
+        <v>4</v>
+      </c>
+      <c r="J31" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="3:10">
+      <c r="E32">
+        <v>5000</v>
+      </c>
+      <c r="H32">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="5:8">
+      <c r="E33">
+        <f>SUMIF(F28:F29,"a",E28:E32)</f>
+        <v>1</v>
+      </c>
+      <c r="H33">
+        <f ca="1">SUMIF(I28:I31,"a",H28)</f>
+        <v>3001</v>
+      </c>
+    </row>
+    <row r="34" spans="5:8">
+      <c r="H34" t="e">
+        <f>SUMIFS(H28:H31,I28:I30,"a",J28:J31,"x")</f>
         <v>#VALUE!</v>
       </c>
     </row>

</xml_diff>

<commit_message>
SUMIF and SUMIFS can now cope with being passed ranges for the criteria
</commit_message>
<xml_diff>
--- a/examples/rangesinsteadofcells.xlsx
+++ b/examples/rangesinsteadofcells.xlsx
@@ -104,8 +104,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="65">
+  <cellStyleXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -179,7 +181,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="65">
+  <cellStyles count="67">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -212,6 +214,7 @@
     <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -244,6 +247,7 @@
     <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -573,10 +577,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B6:O40"/>
+  <dimension ref="B6:O48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H40" sqref="H40"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -644,7 +648,7 @@
         <v>2</v>
       </c>
       <c r="C8" s="1">
-        <f t="shared" ref="C8:H12" si="1">$C$6:$H$6*$B$7:$B$12</f>
+        <f t="shared" ref="C8:C12" si="1">$C$6:$H$6*$B$7:$B$12</f>
         <v>2</v>
       </c>
       <c r="D8" s="1">
@@ -836,72 +840,60 @@
     </row>
     <row r="18" spans="3:14">
       <c r="C18">
-        <f>10/$C$6:$H$6</f>
+        <f t="shared" ref="C18:H18" si="3">10/$C$6:$H$6</f>
         <v>10</v>
       </c>
       <c r="D18">
-        <f>10/$C$6:$H$6</f>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="E18">
-        <f>10/$C$6:$H$6</f>
+        <f t="shared" si="3"/>
         <v>3.3333333333333335</v>
       </c>
       <c r="F18">
-        <f>10/$C$6:$H$6</f>
+        <f t="shared" si="3"/>
         <v>2.5</v>
       </c>
       <c r="G18">
-        <f>10/$C$6:$H$6</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="H18">
-        <f>10/$C$6:$H$6</f>
+        <f t="shared" si="3"/>
         <v>1.6666666666666667</v>
       </c>
     </row>
     <row r="19" spans="3:14">
       <c r="C19">
-        <f>$C$6:$H$6</f>
+        <f t="shared" ref="C19:H19" si="4">$C$6:$H$6</f>
         <v>1</v>
       </c>
       <c r="D19">
-        <f>$C$6:$H$6</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="E19">
-        <f>$C$6:$H$6</f>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="F19">
-        <f>$C$6:$H$6</f>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="G19">
-        <f>$C$6:$H$6</f>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
       <c r="H19">
-        <f>$C$6:$H$6</f>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
     </row>
     <row r="22" spans="3:14">
-      <c r="C22" t="e">
-        <f>$C$7:$H$8</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D22" t="e">
-        <f>$C$6:$E$6+$E$7:$H$7</f>
-        <v>#VALUE!</v>
-      </c>
       <c r="E22">
         <f>$C$6:$E$6+$E$7:$H$7</f>
         <v>6</v>
-      </c>
-      <c r="F22" t="e">
-        <f>$C$6:$E$6+$E$7:$H$7</f>
-        <v>#VALUE!</v>
       </c>
       <c r="K22" t="s">
         <v>6</v>
@@ -1082,7 +1074,7 @@
         <v>1020100</v>
       </c>
     </row>
-    <row r="33" spans="5:15">
+    <row r="33" spans="4:15">
       <c r="E33">
         <f>SUMIF(F28:F29,"a",E28:E32)</f>
         <v>1</v>
@@ -1092,13 +1084,13 @@
         <v>3001</v>
       </c>
     </row>
-    <row r="34" spans="5:15">
+    <row r="34" spans="4:15">
       <c r="H34" t="e">
         <f>SUMIFS(H28:H31,I28:I30,"a",J28:J31,"x")</f>
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="38" spans="5:15">
+    <row r="38" spans="4:15">
       <c r="M38">
         <v>3</v>
       </c>
@@ -1109,7 +1101,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="5:15">
+    <row r="39" spans="4:15">
       <c r="L39">
         <v>4</v>
       </c>
@@ -1122,11 +1114,11 @@
         <v>4</v>
       </c>
       <c r="O39">
-        <f t="array" ref="O39">SUM((Sheet2!$D$13:$G$13=O$38)*(Sheet2!$C$22:$C$25=$L39)*(Sheet2!$D$22:$G$25))</f>
+        <f t="array" ref="O39">SUM(IFERROR((Sheet2!$D$13:$G$13=O$38)*(Sheet2!$C$22:$C$25=$L39)*(Sheet2!$D$22:$G$25),0))</f>
         <v>16</v>
       </c>
     </row>
-    <row r="40" spans="5:15">
+    <row r="40" spans="4:15">
       <c r="F40">
         <f>SUMPRODUCT(B7:B12,B7:B12)</f>
         <v>91</v>
@@ -1150,6 +1142,116 @@
       <c r="O40">
         <f t="array" ref="O40">SUM((Sheet2!$D$13:$G$13=O$38)*(Sheet2!$C$22:$C$25=$L40)*(Sheet2!$D$22:$G$25))</f>
         <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="4:15">
+      <c r="D43">
+        <v>10</v>
+      </c>
+      <c r="E43">
+        <v>1</v>
+      </c>
+      <c r="F43">
+        <v>3</v>
+      </c>
+      <c r="G43">
+        <f>SUMIF($E$43:$E$48,$F$43:$F$48,$D$43:$D$48)</f>
+        <v>30</v>
+      </c>
+      <c r="I43">
+        <f>$F$43:$F$48</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="4:15">
+      <c r="D44">
+        <v>20</v>
+      </c>
+      <c r="E44">
+        <v>2</v>
+      </c>
+      <c r="F44">
+        <v>4</v>
+      </c>
+      <c r="G44">
+        <f>SUMIF($E$43:$E$48,$F$43:$F$48,$D$43:$D$48)</f>
+        <v>40</v>
+      </c>
+      <c r="I44">
+        <f t="shared" ref="I44:I47" si="5">$F$43:$F$48</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="4:15">
+      <c r="D45">
+        <v>30</v>
+      </c>
+      <c r="E45">
+        <v>3</v>
+      </c>
+      <c r="F45">
+        <v>2</v>
+      </c>
+      <c r="G45">
+        <f>SUMIF($E$43:$E$48,$F$43:$F$48,$D$43:$D$48)</f>
+        <v>20</v>
+      </c>
+      <c r="I45">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="4:15">
+      <c r="D46">
+        <v>40</v>
+      </c>
+      <c r="E46">
+        <v>4</v>
+      </c>
+      <c r="F46">
+        <v>1</v>
+      </c>
+      <c r="G46">
+        <f>SUMIF($E$43:$E$48,$F$43:$F$48,$D$43:$D$48)</f>
+        <v>10</v>
+      </c>
+      <c r="I46">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="4:15">
+      <c r="D47">
+        <v>50</v>
+      </c>
+      <c r="E47">
+        <v>5</v>
+      </c>
+      <c r="F47">
+        <v>10</v>
+      </c>
+      <c r="G47">
+        <f>SUMIF($E$43:$E$48,$F$43:$F$48,$D$43:$D$48)</f>
+        <v>0</v>
+      </c>
+      <c r="I47">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="48" spans="4:15">
+      <c r="D48">
+        <v>60</v>
+      </c>
+      <c r="E48">
+        <v>6</v>
+      </c>
+      <c r="F48">
+        <v>0</v>
+      </c>
+      <c r="G48">
+        <f>SUMIF($E$43:$E$48,$F$43:$F$48,$D$43:$D$48)</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1224,19 +1326,19 @@
         <v>1</v>
       </c>
       <c r="D22">
-        <f>$C22*D$13</f>
+        <f t="shared" ref="D22:G25" si="0">$C22*D$13</f>
         <v>1</v>
       </c>
       <c r="E22">
-        <f>$C22*E$13</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="F22">
-        <f>$C22*F$13</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="G22">
-        <f>$C22*G$13</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
@@ -1245,19 +1347,19 @@
         <v>2</v>
       </c>
       <c r="D23">
-        <f>$C23*D$13</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="E23">
-        <f>$C23*E$13</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="F23">
-        <f>$C23*F$13</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="G23">
-        <f>$C23*G$13</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
@@ -1266,19 +1368,19 @@
         <v>3</v>
       </c>
       <c r="D24">
-        <f>$C24*D$13</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="E24">
-        <f>$C24*E$13</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="F24">
-        <f>$C24*F$13</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="G24">
-        <f>$C24*G$13</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
     </row>
@@ -1287,19 +1389,19 @@
         <v>4</v>
       </c>
       <c r="D25">
-        <f>$C25*D$13</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="E25">
-        <f>$C25*E$13</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="F25">
-        <f>$C25*F$13</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="G25">
-        <f>$C25*G$13</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
     </row>

</xml_diff>

<commit_message>
INDEX can now work with ranges passed as its second and/or third arguments
</commit_message>
<xml_diff>
--- a/examples/rangesinsteadofcells.xlsx
+++ b/examples/rangesinsteadofcells.xlsx
@@ -1,16 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10311"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tamc/Documents/github/excel_to_code/examples/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3A09265-8D8A-C54C-9412-AA83B73CDEBE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="17240" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="440" windowWidth="25360" windowHeight="17240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140000" calcMode="manual" concurrentCalc="0"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -55,7 +61,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -252,6 +258,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -576,16 +590,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B6:O48"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B6:O55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="B24" workbookViewId="0">
+      <selection activeCell="H55" sqref="H55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="6" spans="2:14">
+    <row r="6" spans="2:14" x14ac:dyDescent="0.2">
       <c r="C6">
         <v>1</v>
       </c>
@@ -605,7 +619,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="2:14">
+    <row r="7" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B7">
         <v>1</v>
       </c>
@@ -643,7 +657,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:14">
+    <row r="8" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B8">
         <v>2</v>
       </c>
@@ -678,7 +692,7 @@
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
     </row>
-    <row r="9" spans="2:14">
+    <row r="9" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B9">
         <v>3</v>
       </c>
@@ -713,7 +727,7 @@
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
     </row>
-    <row r="10" spans="2:14">
+    <row r="10" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B10">
         <v>4</v>
       </c>
@@ -748,7 +762,7 @@
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
     </row>
-    <row r="11" spans="2:14">
+    <row r="11" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B11">
         <v>5</v>
       </c>
@@ -777,7 +791,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="2:14">
+    <row r="12" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B12">
         <v>6</v>
       </c>
@@ -806,13 +820,13 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="2:14">
+    <row r="14" spans="2:14" x14ac:dyDescent="0.2">
       <c r="C14" s="1">
         <f>SUM($C$6:$H$6)</f>
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="2:14">
+    <row r="15" spans="2:14" x14ac:dyDescent="0.2">
       <c r="C15">
         <f t="shared" ref="C15:H15" si="2">C6:H6</f>
         <v>1</v>
@@ -838,7 +852,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="3:14">
+    <row r="18" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C18">
         <f t="shared" ref="C18:H18" si="3">10/$C$6:$H$6</f>
         <v>10</v>
@@ -864,7 +878,7 @@
         <v>1.6666666666666667</v>
       </c>
     </row>
-    <row r="19" spans="3:14">
+    <row r="19" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C19">
         <f t="shared" ref="C19:H19" si="4">$C$6:$H$6</f>
         <v>1</v>
@@ -890,7 +904,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="3:14">
+    <row r="22" spans="3:14" x14ac:dyDescent="0.2">
       <c r="E22">
         <f>$C$6:$E$6+$E$7:$H$7</f>
         <v>6</v>
@@ -909,7 +923,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="23" spans="3:14">
+    <row r="23" spans="3:14" x14ac:dyDescent="0.2">
       <c r="K23" t="s">
         <v>7</v>
       </c>
@@ -920,7 +934,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="3:14">
+    <row r="24" spans="3:14" x14ac:dyDescent="0.2">
       <c r="K24" t="s">
         <v>6</v>
       </c>
@@ -931,7 +945,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="3:14">
+    <row r="25" spans="3:14" x14ac:dyDescent="0.2">
       <c r="K25" t="s">
         <v>7</v>
       </c>
@@ -942,7 +956,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="3:14">
+    <row r="26" spans="3:14" x14ac:dyDescent="0.2">
       <c r="K26" t="s">
         <v>6</v>
       </c>
@@ -957,7 +971,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="27" spans="3:14">
+    <row r="27" spans="3:14" x14ac:dyDescent="0.2">
       <c r="K27" t="s">
         <v>7</v>
       </c>
@@ -968,7 +982,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="3:14">
+    <row r="28" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C28">
         <f>SUMPRODUCT(B7:B12,B7:B12)</f>
         <v>91</v>
@@ -993,7 +1007,7 @@
         <v>1260</v>
       </c>
     </row>
-    <row r="29" spans="3:14">
+    <row r="29" spans="3:14" x14ac:dyDescent="0.2">
       <c r="E29">
         <v>2</v>
       </c>
@@ -1020,7 +1034,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="3:14">
+    <row r="30" spans="3:14" x14ac:dyDescent="0.2">
       <c r="E30">
         <v>3</v>
       </c>
@@ -1041,7 +1055,7 @@
         <v>50500</v>
       </c>
     </row>
-    <row r="31" spans="3:14">
+    <row r="31" spans="3:14" x14ac:dyDescent="0.2">
       <c r="E31">
         <v>4</v>
       </c>
@@ -1058,7 +1072,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="3:14">
+    <row r="32" spans="3:14" x14ac:dyDescent="0.2">
       <c r="E32">
         <v>5000</v>
       </c>
@@ -1074,7 +1088,7 @@
         <v>1020100</v>
       </c>
     </row>
-    <row r="33" spans="4:15">
+    <row r="33" spans="4:15" x14ac:dyDescent="0.2">
       <c r="E33">
         <f>SUMIF(F28:F29,"a",E28:E32)</f>
         <v>1</v>
@@ -1084,13 +1098,13 @@
         <v>3001</v>
       </c>
     </row>
-    <row r="34" spans="4:15">
+    <row r="34" spans="4:15" x14ac:dyDescent="0.2">
       <c r="H34" t="e">
         <f>SUMIFS(H28:H31,I28:I30,"a",J28:J31,"x")</f>
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="38" spans="4:15">
+    <row r="38" spans="4:15" x14ac:dyDescent="0.2">
       <c r="M38">
         <v>3</v>
       </c>
@@ -1101,7 +1115,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="4:15">
+    <row r="39" spans="4:15" x14ac:dyDescent="0.2">
       <c r="L39">
         <v>4</v>
       </c>
@@ -1118,7 +1132,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="40" spans="4:15">
+    <row r="40" spans="4:15" x14ac:dyDescent="0.2">
       <c r="F40">
         <f>SUMPRODUCT(B7:B12,B7:B12)</f>
         <v>91</v>
@@ -1144,7 +1158,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="4:15">
+    <row r="43" spans="4:15" x14ac:dyDescent="0.2">
       <c r="D43">
         <v>10</v>
       </c>
@@ -1155,7 +1169,7 @@
         <v>3</v>
       </c>
       <c r="G43">
-        <f>SUMIF($E$43:$E$48,$F$43:$F$48,$D$43:$D$48)</f>
+        <f t="shared" ref="G43:G48" si="5">SUMIF($E$43:$E$48,$F$43:$F$48,$D$43:$D$48)</f>
         <v>30</v>
       </c>
       <c r="I43">
@@ -1163,7 +1177,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="4:15">
+    <row r="44" spans="4:15" x14ac:dyDescent="0.2">
       <c r="D44">
         <v>20</v>
       </c>
@@ -1174,15 +1188,15 @@
         <v>4</v>
       </c>
       <c r="G44">
-        <f>SUMIF($E$43:$E$48,$F$43:$F$48,$D$43:$D$48)</f>
+        <f t="shared" si="5"/>
         <v>40</v>
       </c>
       <c r="I44">
-        <f t="shared" ref="I44:I47" si="5">$F$43:$F$48</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="45" spans="4:15">
+        <f t="shared" ref="I44:I47" si="6">$F$43:$F$48</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="4:15" x14ac:dyDescent="0.2">
       <c r="D45">
         <v>30</v>
       </c>
@@ -1193,15 +1207,15 @@
         <v>2</v>
       </c>
       <c r="G45">
-        <f>SUMIF($E$43:$E$48,$F$43:$F$48,$D$43:$D$48)</f>
+        <f t="shared" si="5"/>
         <v>20</v>
       </c>
       <c r="I45">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="46" spans="4:15">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="4:15" x14ac:dyDescent="0.2">
       <c r="D46">
         <v>40</v>
       </c>
@@ -1212,15 +1226,15 @@
         <v>1</v>
       </c>
       <c r="G46">
-        <f>SUMIF($E$43:$E$48,$F$43:$F$48,$D$43:$D$48)</f>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="I46">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="4:15">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="4:15" x14ac:dyDescent="0.2">
       <c r="D47">
         <v>50</v>
       </c>
@@ -1231,15 +1245,15 @@
         <v>10</v>
       </c>
       <c r="G47">
-        <f>SUMIF($E$43:$E$48,$F$43:$F$48,$D$43:$D$48)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="I47">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
     </row>
-    <row r="48" spans="4:15">
+    <row r="48" spans="4:15" x14ac:dyDescent="0.2">
       <c r="D48">
         <v>60</v>
       </c>
@@ -1250,8 +1264,64 @@
         <v>0</v>
       </c>
       <c r="G48">
-        <f>SUMIF($E$43:$E$48,$F$43:$F$48,$D$43:$D$48)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="D53">
+        <v>10</v>
+      </c>
+      <c r="E53">
+        <v>20</v>
+      </c>
+      <c r="F53">
+        <v>30</v>
+      </c>
+      <c r="G53">
+        <v>40</v>
+      </c>
+      <c r="H53">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="54" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="D54">
+        <v>5</v>
+      </c>
+      <c r="E54">
+        <v>4</v>
+      </c>
+      <c r="F54">
+        <v>3</v>
+      </c>
+      <c r="G54">
+        <v>2</v>
+      </c>
+      <c r="H54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="D55">
+        <f>INDEX($D$53:$H$53,1,$D$54:$H$54)</f>
+        <v>50</v>
+      </c>
+      <c r="E55">
+        <f t="shared" ref="E55:H55" si="7">INDEX($D$53:$H$53,1,$D$54:$H$54)</f>
+        <v>40</v>
+      </c>
+      <c r="F55">
+        <f t="shared" si="7"/>
+        <v>30</v>
+      </c>
+      <c r="G55">
+        <f t="shared" si="7"/>
+        <v>20</v>
+      </c>
+      <c r="H55">
+        <f t="shared" si="7"/>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -1266,16 +1336,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="C4:G25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D22" sqref="D22:G25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="4" spans="4:7">
+    <row r="4" spans="4:7" x14ac:dyDescent="0.2">
       <c r="D4">
         <v>1</v>
       </c>
@@ -1289,7 +1359,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="4:7">
+    <row r="5" spans="4:7" x14ac:dyDescent="0.2">
       <c r="D5">
         <f>$D$4:$G$4</f>
         <v>1</v>
@@ -1307,7 +1377,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="4:7">
+    <row r="13" spans="4:7" x14ac:dyDescent="0.2">
       <c r="D13">
         <v>1</v>
       </c>
@@ -1321,7 +1391,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="3:7">
+    <row r="22" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C22">
         <v>1</v>
       </c>
@@ -1342,7 +1412,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="3:7">
+    <row r="23" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C23">
         <v>2</v>
       </c>
@@ -1363,7 +1433,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="3:7">
+    <row r="24" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C24">
         <v>3</v>
       </c>
@@ -1384,7 +1454,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="3:7">
+    <row r="25" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C25">
         <v>4</v>
       </c>

</xml_diff>